<commit_message>
Pushing updated graphs for archive experiments
</commit_message>
<xml_diff>
--- a/graphs/archiveRunnings.xlsx
+++ b/graphs/archiveRunnings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="20">
   <si>
     <t>6 month</t>
   </si>
@@ -57,9 +57,6 @@
     <t>month</t>
   </si>
   <si>
-    <t>  </t>
-  </si>
-  <si>
     <t>Last year</t>
   </si>
   <si>
@@ -79,6 +76,7 @@
         <color rgb="FF000000"/>
         <rFont val="Liberation Sans1"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">wo</t>
     </r>
@@ -88,6 +86,7 @@
         <color rgb="FF000000"/>
         <rFont val="Liberation Sans1"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Year</t>
     </r>
@@ -109,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -138,14 +137,10 @@
       <color rgb="FF000000"/>
       <name val="Liberation Sans1"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Liberation Sans1"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <b val="true"/>
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -156,6 +151,7 @@
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -267,7 +263,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -280,7 +276,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -294,7 +290,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>6 month</a:t>
@@ -312,17 +308,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>kr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="004586"/>
@@ -337,390 +322,13 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:xVal>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>112.861783113739</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>176.109549117227</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>224.35812347551</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>345.209950867179</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>411.802046262694</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>473.131746135373</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>623.23880769668</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>530.983323413438</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>727.788831614565</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>681.754080205969</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>976.445551681484</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>766.322393605698</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1035.01988286818</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1084.88798114909</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1375.83647872271</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1030.14477595894</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1755.86386426634</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1076.89578187415</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1651.4026836394</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>0.485725140154162</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.438500740874629</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.397838282608353</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.387925730688704</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.338124732135973</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.311408099922318</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.310497201862126</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.322220411580731</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.315910272464974</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.302037109990771</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.264603681766873</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.288340596944481</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.239978561781693</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.256956782235666</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.253573742093923</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.290629307284112</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.214839781565726</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.278300530445386</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.209992068423969</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>label 3</c:f>
+              <c:f>label 0</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -743,134 +351,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>2</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -996,7 +479,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>3</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -1126,7 +609,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>label 5</c:f>
+              <c:f>label 2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1149,134 +632,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>4</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -1402,7 +760,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>5</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -1532,7 +890,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>label 7</c:f>
+              <c:f>label 4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1555,134 +913,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>6</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -1808,7 +1041,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>7</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -1933,11 +1166,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91885425"/>
-        <c:axId val="24730365"/>
+        <c:axId val="14831312"/>
+        <c:axId val="17235642"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91885425"/>
+        <c:axId val="14831312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1953,7 +1186,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Avg Block Size
@@ -1974,11 +1207,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="24730365"/>
+        <c:crossAx val="17235642"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="24730365"/>
+        <c:axId val="17235642"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2003,7 +1236,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Ratio</a:t>
@@ -2023,7 +1256,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91885425"/>
+        <c:crossAx val="14831312"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2058,7 +1291,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2072,7 +1305,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Last year</a:t>
@@ -2090,17 +1323,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>kr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="004586"/>
@@ -2115,390 +1337,13 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:xVal>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>112.861783113739</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>176.109549117227</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>224.35812347551</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>345.209950867179</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>411.802046262694</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>473.131746135373</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>623.23880769668</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>530.983323413438</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>727.788831614565</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>681.754080205969</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>976.445551681484</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>766.322393605698</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1035.01988286818</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1084.88798114909</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1375.83647872271</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1030.14477595894</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1755.86386426634</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1076.89578187415</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1651.4026836394</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>0.428272326572729</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.385876588121452</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.353007845813315</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.347282317066449</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.297932317602367</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.276589577977257</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.277768813354587</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.286310798589883</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.286869227161129</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.273790771550553</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.236310398533084</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.259309436317052</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.214271338882729</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.231407548474659</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.230610511082794</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.267020539513518</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.194149869281921</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.255940293819594</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.189772519965457</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>label 3</c:f>
+              <c:f>label 0</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2521,134 +1366,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>2</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -2774,7 +1494,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>3</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -2904,7 +1624,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>label 5</c:f>
+              <c:f>label 2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2927,134 +1647,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>4</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -3180,7 +1775,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>5</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -3310,7 +1905,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>label 7</c:f>
+              <c:f>label 4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3333,134 +1928,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>6</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -3586,7 +2056,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>7</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -3711,11 +2181,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="59489700"/>
-        <c:axId val="23227034"/>
+        <c:axId val="53544160"/>
+        <c:axId val="48609661"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59489700"/>
+        <c:axId val="53544160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3731,7 +2201,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Avg Block Size</a:t>
@@ -3751,11 +2221,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="23227034"/>
+        <c:crossAx val="48609661"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="23227034"/>
+        <c:axId val="48609661"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3780,7 +2250,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Ratio</a:t>
@@ -3800,7 +2270,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="59489700"/>
+        <c:crossAx val="53544160"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3835,7 +2305,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3849,7 +2319,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>2 years</a:t>
@@ -3867,17 +2337,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>kr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="004586"/>
@@ -3892,390 +2351,13 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:xVal>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>112.861783113739</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>176.109549117227</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>224.35812347551</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>345.209950867179</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>411.802046262694</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>473.131746135373</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>623.23880769668</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>530.983323413438</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>727.788831614565</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>681.754080205969</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>976.445551681484</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>766.322393605698</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1035.01988286818</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1084.88798114909</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1375.83647872271</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1030.14477595894</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1755.86386426634</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1076.89578187415</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1651.4026836394</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>0.362543775926307</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.329102310758445</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.30342882788652</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.302006707641546</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.258025336315728</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.239172231813217</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.241988239479706</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.25255081761106</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.25445105222477</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.243653134958312</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.208273577431433</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.229993847734198</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.1881533037845</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.206426475652408</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.204503399367401</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.241278122993551</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.17325167328997</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.23284996103454</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.168750446555447</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>label 3</c:f>
+              <c:f>label 0</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4298,134 +2380,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>2</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -4551,7 +2508,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>3</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -4681,7 +2638,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>label 5</c:f>
+              <c:f>label 2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4704,134 +2661,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>4</c:f>
+              <c:f>3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -4957,7 +2789,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>5</c:f>
+              <c:f>2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -5087,7 +2919,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>label 7</c:f>
+              <c:f>label 4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5110,134 +2942,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:xVal>
             <c:numRef>
-              <c:f>6</c:f>
+              <c:f>5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -5363,7 +3070,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>7</c:f>
+              <c:f>4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -5488,11 +3195,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="58913233"/>
-        <c:axId val="83996616"/>
+        <c:axId val="98137645"/>
+        <c:axId val="74965072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58913233"/>
+        <c:axId val="98137645"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5508,7 +3215,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Avg Block Size</a:t>
@@ -5528,11 +3235,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="83996616"/>
+        <c:crossAx val="74965072"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83996616"/>
+        <c:axId val="74965072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5557,7 +3264,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Ratio</a:t>
@@ -5577,7 +3284,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="58913233"/>
+        <c:crossAx val="98137645"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -5617,15 +3324,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>138600</xdr:colOff>
+      <xdr:colOff>192600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>559800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:colOff>613080</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5633,8 +3340,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15310440" y="105840"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="15364440" y="87840"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5647,15 +3354,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>131040</xdr:colOff>
+      <xdr:colOff>185040</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>43920</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>552240</xdr:colOff>
+      <xdr:colOff>605520</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5663,8 +3370,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15302880" y="4425120"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="15356880" y="4407120"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5676,16 +3383,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>742320</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>33840</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>401040</xdr:colOff>
+      <xdr:colOff>454320</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>164160</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5693,8 +3400,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15151680" y="7965720"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="15205680" y="7947720"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5712,10 +3419,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R127"/>
+  <dimension ref="A1:O127"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="1" sqref="E100:G100 O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6405,9 +4112,6 @@
       <c r="O18" s="0" t="n">
         <v>0.290629307284112</v>
       </c>
-      <c r="R18" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -6745,22 +4449,22 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I45" s="0" t="s">
         <v>11</v>
       </c>
       <c r="J45" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K45" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K45" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="M45" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7736,10 +5440,10 @@
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="E87" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7768,10 +5472,10 @@
         <v>2</v>
       </c>
       <c r="K88" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M88" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="M88" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8742,10 +6446,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O107"/>
+  <dimension ref="A1:Q107"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E100" activeCellId="0" sqref="E100:G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -8757,8 +6461,10 @@
     <col collapsed="false" hidden="false" max="11" min="9" style="0" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6275303643725"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.995951417004"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="10.6275303643725"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6275303643725"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.995951417004"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="10.6275303643725"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8783,10 +6489,10 @@
       <c r="K1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -8818,13 +6524,13 @@
       <c r="K2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -8851,18 +6557,24 @@
         <v>100</v>
       </c>
       <c r="J3" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>251</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>305.769928971697</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="M3" s="0" t="n">
         <v>0.405559272262192</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="O3" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="P3" s="0" t="n">
         <v>103.494720238677</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="Q3" s="0" t="n">
         <v>0.524511674036988</v>
       </c>
     </row>
@@ -8889,18 +6601,24 @@
         <v>150</v>
       </c>
       <c r="J4" s="0" t="n">
+        <v>751</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>371</v>
+      </c>
+      <c r="L4" s="0" t="n">
         <v>466.931199458631</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="M4" s="0" t="n">
         <v>0.363581804649185</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="O4" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="P4" s="0" t="n">
         <v>161.990429809269</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="Q4" s="0" t="n">
         <v>0.454353654971457</v>
       </c>
     </row>
@@ -8927,18 +6645,24 @@
         <v>200</v>
       </c>
       <c r="J5" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="L5" s="0" t="n">
         <v>600.581242611654</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="M5" s="0" t="n">
         <v>0.340595468812963</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="O5" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="P5" s="0" t="n">
         <v>192.810214544067</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="Q5" s="0" t="n">
         <v>0.437017143892992</v>
       </c>
     </row>
@@ -8965,18 +6689,24 @@
         <v>250</v>
       </c>
       <c r="J6" s="0" t="n">
+        <v>1251</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>621</v>
+      </c>
+      <c r="L6" s="0" t="n">
         <v>814.758063919752</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="M6" s="0" t="n">
         <v>0.305255160635546</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="O6" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="P6" s="0" t="n">
         <v>287.491706423398</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="Q6" s="0" t="n">
         <v>0.397547480685012</v>
       </c>
     </row>
@@ -9003,18 +6733,24 @@
         <v>300</v>
       </c>
       <c r="J7" s="0" t="n">
+        <v>1501</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>751</v>
+      </c>
+      <c r="L7" s="0" t="n">
         <v>1052.03854317287</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="M7" s="0" t="n">
         <v>0.286395947864871</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="O7" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="P7" s="0" t="n">
         <v>419.512827506846</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="Q7" s="0" t="n">
         <v>0.378198995955275</v>
       </c>
     </row>
@@ -9041,18 +6777,24 @@
         <v>350</v>
       </c>
       <c r="J8" s="0" t="n">
+        <v>1751</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>871</v>
+      </c>
+      <c r="L8" s="0" t="n">
         <v>1124.99284950306</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="M8" s="0" t="n">
         <v>0.284473733338499</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="O8" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="P8" s="0" t="n">
         <v>423.055158924448</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="Q8" s="0" t="n">
         <v>0.355880078689699</v>
       </c>
     </row>
@@ -9079,18 +6821,24 @@
         <v>400</v>
       </c>
       <c r="J9" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="L9" s="0" t="n">
         <v>1206.63863671213</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="M9" s="0" t="n">
         <v>0.267867386666292</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="O9" s="0" t="n">
         <v>400</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="P9" s="0" t="n">
         <v>418.269533888814</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="Q9" s="0" t="n">
         <v>0.334351888176728</v>
       </c>
     </row>
@@ -9117,18 +6865,24 @@
         <v>450</v>
       </c>
       <c r="J10" s="0" t="n">
+        <v>2251</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>1121</v>
+      </c>
+      <c r="L10" s="0" t="n">
         <v>1557.05233674074</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="M10" s="0" t="n">
         <v>0.236738559928588</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="O10" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="P10" s="0" t="n">
         <v>614.088661374743</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="Q10" s="0" t="n">
         <v>0.293941391925161</v>
       </c>
     </row>
@@ -9155,18 +6909,24 @@
         <v>500</v>
       </c>
       <c r="J11" s="0" t="n">
+        <v>2501</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>1251</v>
+      </c>
+      <c r="L11" s="0" t="n">
         <v>1651.41076873964</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="M11" s="0" t="n">
         <v>0.251651055385142</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="O11" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="P11" s="0" t="n">
         <v>585.854118922896</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="Q11" s="0" t="n">
         <v>0.35023175949554</v>
       </c>
     </row>
@@ -9193,18 +6953,24 @@
         <v>550</v>
       </c>
       <c r="J12" s="0" t="n">
+        <v>2751</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>1371</v>
+      </c>
+      <c r="L12" s="0" t="n">
         <v>1830.78323536227</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="M12" s="0" t="n">
         <v>0.248144509204521</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="O12" s="0" t="n">
         <v>550</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="P12" s="0" t="n">
         <v>696.627465616338</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="Q12" s="0" t="n">
         <v>0.33894558289428</v>
       </c>
     </row>
@@ -9231,18 +6997,24 @@
         <v>600</v>
       </c>
       <c r="J13" s="0" t="n">
+        <v>3001</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>1501</v>
+      </c>
+      <c r="L13" s="0" t="n">
         <v>2067.42872491427</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="M13" s="0" t="n">
         <v>0.245708112562289</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="O13" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="P13" s="0" t="n">
         <v>772.806145217572</v>
       </c>
-      <c r="O13" s="0" t="n">
+      <c r="Q13" s="0" t="n">
         <v>0.313021237008312</v>
       </c>
     </row>
@@ -9269,18 +7041,24 @@
         <v>650</v>
       </c>
       <c r="J14" s="0" t="n">
+        <v>3251</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>1621</v>
+      </c>
+      <c r="L14" s="0" t="n">
         <v>2175.41215308844</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="M14" s="0" t="n">
         <v>0.22511343919814</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="O14" s="0" t="n">
         <v>650</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="P14" s="0" t="n">
         <v>805.845856011652</v>
       </c>
-      <c r="O14" s="0" t="n">
+      <c r="Q14" s="0" t="n">
         <v>0.294676528668462</v>
       </c>
     </row>
@@ -9307,18 +7085,24 @@
         <v>700</v>
       </c>
       <c r="J15" s="0" t="n">
+        <v>3501</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>1751</v>
+      </c>
+      <c r="L15" s="0" t="n">
         <v>2308.71035744086</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="M15" s="0" t="n">
         <v>0.232369594350125</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="O15" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="P15" s="0" t="n">
         <v>882.740871570471</v>
       </c>
-      <c r="O15" s="0" t="n">
+      <c r="Q15" s="0" t="n">
         <v>0.280827299518328</v>
       </c>
     </row>
@@ -9345,18 +7129,24 @@
         <v>750</v>
       </c>
       <c r="J16" s="0" t="n">
+        <v>3751</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>1871</v>
+      </c>
+      <c r="L16" s="0" t="n">
         <v>2408.50395588857</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="M16" s="0" t="n">
         <v>0.225183264504556</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="O16" s="0" t="n">
         <v>750</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="P16" s="0" t="n">
         <v>892.100722151325</v>
       </c>
-      <c r="O16" s="0" t="n">
+      <c r="Q16" s="0" t="n">
         <v>0.289484490580728</v>
       </c>
     </row>
@@ -9383,18 +7173,24 @@
         <v>800</v>
       </c>
       <c r="J17" s="0" t="n">
+        <v>4001</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="L17" s="0" t="n">
         <v>2591.11926901876</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="M17" s="0" t="n">
         <v>0.198427923038837</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="O17" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="P17" s="0" t="n">
         <v>826.838214050031</v>
       </c>
-      <c r="O17" s="0" t="n">
+      <c r="Q17" s="0" t="n">
         <v>0.273491002240484</v>
       </c>
     </row>
@@ -9421,18 +7217,24 @@
         <v>850</v>
       </c>
       <c r="J18" s="0" t="n">
+        <v>4251</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>2121</v>
+      </c>
+      <c r="L18" s="0" t="n">
         <v>2907.32613443273</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="M18" s="0" t="n">
         <v>0.19455362717264</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="O18" s="0" t="n">
         <v>850</v>
       </c>
-      <c r="N18" s="0" t="n">
+      <c r="P18" s="0" t="n">
         <v>1044.66558142264</v>
       </c>
-      <c r="O18" s="0" t="n">
+      <c r="Q18" s="0" t="n">
         <v>0.270593488229482</v>
       </c>
     </row>
@@ -9459,18 +7261,24 @@
         <v>900</v>
       </c>
       <c r="J19" s="0" t="n">
+        <v>4501</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>2251</v>
+      </c>
+      <c r="L19" s="0" t="n">
         <v>3213.15662929119</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="M19" s="0" t="n">
         <v>0.182660689632835</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="O19" s="0" t="n">
         <v>900</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="P19" s="0" t="n">
         <v>1243.08363246114</v>
       </c>
-      <c r="O19" s="0" t="n">
+      <c r="Q19" s="0" t="n">
         <v>0.253402141670243</v>
       </c>
     </row>
@@ -9497,18 +7305,24 @@
         <v>950</v>
       </c>
       <c r="J20" s="0" t="n">
+        <v>4751</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>2371</v>
+      </c>
+      <c r="L20" s="0" t="n">
         <v>3226.15301186036</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="M20" s="0" t="n">
         <v>0.185185077744198</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="O20" s="0" t="n">
         <v>950</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="P20" s="0" t="n">
         <v>1295.51961245325</v>
       </c>
-      <c r="O20" s="0" t="n">
+      <c r="Q20" s="0" t="n">
         <v>0.246100668521059</v>
       </c>
     </row>
@@ -9535,39 +7349,45 @@
         <v>1000</v>
       </c>
       <c r="J21" s="0" t="n">
+        <v>5001</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>2501</v>
+      </c>
+      <c r="L21" s="0" t="n">
         <v>3248.84490838425</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="M21" s="0" t="n">
         <v>0.203030565199311</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="O21" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="N21" s="0" t="n">
+      <c r="P21" s="0" t="n">
         <v>1148.49410646982</v>
       </c>
-      <c r="O21" s="0" t="n">
+      <c r="Q21" s="0" t="n">
         <v>0.275706894407989</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I45" s="0" t="s">
         <v>11</v>
       </c>
       <c r="J45" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K45" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="K45" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="M45" s="0" t="s">
-        <v>14</v>
+      <c r="O45" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9589,13 +7409,13 @@
       <c r="G46" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="M46" s="0" t="s">
+      <c r="O46" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="N46" s="0" t="s">
+      <c r="P46" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="O46" s="0" t="s">
+      <c r="Q46" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -9622,18 +7442,24 @@
         <v>100</v>
       </c>
       <c r="J47" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <v>251</v>
+      </c>
+      <c r="L47" s="0" t="n">
         <v>305.769928971697</v>
       </c>
-      <c r="K47" s="0" t="n">
+      <c r="M47" s="0" t="n">
         <v>0.359041842342567</v>
       </c>
-      <c r="M47" s="0" t="n">
+      <c r="O47" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="N47" s="0" t="n">
+      <c r="P47" s="0" t="n">
         <v>103.494720238677</v>
       </c>
-      <c r="O47" s="0" t="n">
+      <c r="Q47" s="0" t="n">
         <v>0.466523906574263</v>
       </c>
     </row>
@@ -9660,18 +7486,24 @@
         <v>150</v>
       </c>
       <c r="J48" s="0" t="n">
+        <v>751</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <v>371</v>
+      </c>
+      <c r="L48" s="0" t="n">
         <v>466.931199458631</v>
       </c>
-      <c r="K48" s="0" t="n">
+      <c r="M48" s="0" t="n">
         <v>0.324942017647884</v>
       </c>
-      <c r="M48" s="0" t="n">
+      <c r="O48" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="N48" s="0" t="n">
+      <c r="P48" s="0" t="n">
         <v>161.990429809269</v>
       </c>
-      <c r="O48" s="0" t="n">
+      <c r="Q48" s="0" t="n">
         <v>0.405395180641114</v>
       </c>
     </row>
@@ -9698,18 +7530,24 @@
         <v>200</v>
       </c>
       <c r="J49" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="K49" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="L49" s="0" t="n">
         <v>600.581242611654</v>
       </c>
-      <c r="K49" s="0" t="n">
+      <c r="M49" s="0" t="n">
         <v>0.306389026884605</v>
       </c>
-      <c r="M49" s="0" t="n">
+      <c r="O49" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="N49" s="0" t="n">
+      <c r="P49" s="0" t="n">
         <v>192.810214544067</v>
       </c>
-      <c r="O49" s="0" t="n">
+      <c r="Q49" s="0" t="n">
         <v>0.390873265576145</v>
       </c>
     </row>
@@ -9736,18 +7574,24 @@
         <v>250</v>
       </c>
       <c r="J50" s="0" t="n">
+        <v>1251</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>621</v>
+      </c>
+      <c r="L50" s="0" t="n">
         <v>814.758063919752</v>
       </c>
-      <c r="K50" s="0" t="n">
+      <c r="M50" s="0" t="n">
         <v>0.274635531596993</v>
       </c>
-      <c r="M50" s="0" t="n">
+      <c r="O50" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="N50" s="0" t="n">
+      <c r="P50" s="0" t="n">
         <v>287.491706423398</v>
       </c>
-      <c r="O50" s="0" t="n">
+      <c r="Q50" s="0" t="n">
         <v>0.357035870121853</v>
       </c>
     </row>
@@ -9774,18 +7618,24 @@
         <v>300</v>
       </c>
       <c r="J51" s="0" t="n">
+        <v>1501</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <v>751</v>
+      </c>
+      <c r="L51" s="0" t="n">
         <v>1052.03854317287</v>
       </c>
-      <c r="K51" s="0" t="n">
+      <c r="M51" s="0" t="n">
         <v>0.257577125371771</v>
       </c>
-      <c r="M51" s="0" t="n">
+      <c r="O51" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="N51" s="0" t="n">
+      <c r="P51" s="0" t="n">
         <v>419.512827506846</v>
       </c>
-      <c r="O51" s="0" t="n">
+      <c r="Q51" s="0" t="n">
         <v>0.339427030023287</v>
       </c>
     </row>
@@ -9812,18 +7662,24 @@
         <v>350</v>
       </c>
       <c r="J52" s="0" t="n">
+        <v>1751</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <v>871</v>
+      </c>
+      <c r="L52" s="0" t="n">
         <v>1124.99284950306</v>
       </c>
-      <c r="K52" s="0" t="n">
+      <c r="M52" s="0" t="n">
         <v>0.2609573344071</v>
       </c>
-      <c r="M52" s="0" t="n">
+      <c r="O52" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="N52" s="0" t="n">
+      <c r="P52" s="0" t="n">
         <v>423.055158924448</v>
       </c>
-      <c r="O52" s="0" t="n">
+      <c r="Q52" s="0" t="n">
         <v>0.319778068286873</v>
       </c>
     </row>
@@ -9850,18 +7706,24 @@
         <v>400</v>
       </c>
       <c r="J53" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="L53" s="0" t="n">
         <v>1206.63863671213</v>
       </c>
-      <c r="K53" s="0" t="n">
+      <c r="M53" s="0" t="n">
         <v>0.241023011482487</v>
       </c>
-      <c r="M53" s="0" t="n">
+      <c r="O53" s="0" t="n">
         <v>400</v>
       </c>
-      <c r="N53" s="0" t="n">
+      <c r="P53" s="0" t="n">
         <v>418.269533888814</v>
       </c>
-      <c r="O53" s="0" t="n">
+      <c r="Q53" s="0" t="n">
         <v>0.301568824709643</v>
       </c>
     </row>
@@ -9888,18 +7750,24 @@
         <v>450</v>
       </c>
       <c r="J54" s="0" t="n">
+        <v>2251</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <v>1121</v>
+      </c>
+      <c r="L54" s="0" t="n">
         <v>1557.05233674074</v>
       </c>
-      <c r="K54" s="0" t="n">
+      <c r="M54" s="0" t="n">
         <v>0.213691429611979</v>
       </c>
-      <c r="M54" s="0" t="n">
+      <c r="O54" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="N54" s="0" t="n">
+      <c r="P54" s="0" t="n">
         <v>614.088661374743</v>
       </c>
-      <c r="O54" s="0" t="n">
+      <c r="Q54" s="0" t="n">
         <v>0.263743657648758</v>
       </c>
     </row>
@@ -9926,18 +7794,24 @@
         <v>500</v>
       </c>
       <c r="J55" s="0" t="n">
+        <v>2501</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <v>1251</v>
+      </c>
+      <c r="L55" s="0" t="n">
         <v>1651.41076873964</v>
       </c>
-      <c r="K55" s="0" t="n">
+      <c r="M55" s="0" t="n">
         <v>0.229254313602245</v>
       </c>
-      <c r="M55" s="0" t="n">
+      <c r="O55" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="N55" s="0" t="n">
+      <c r="P55" s="0" t="n">
         <v>585.854118922896</v>
       </c>
-      <c r="O55" s="0" t="n">
+      <c r="Q55" s="0" t="n">
         <v>0.318479881855447</v>
       </c>
     </row>
@@ -9964,18 +7838,24 @@
         <v>550</v>
       </c>
       <c r="J56" s="0" t="n">
+        <v>2751</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <v>1371</v>
+      </c>
+      <c r="L56" s="0" t="n">
         <v>1830.78323536227</v>
       </c>
-      <c r="K56" s="0" t="n">
+      <c r="M56" s="0" t="n">
         <v>0.228086011158845</v>
       </c>
-      <c r="M56" s="0" t="n">
+      <c r="O56" s="0" t="n">
         <v>550</v>
       </c>
-      <c r="N56" s="0" t="n">
+      <c r="P56" s="0" t="n">
         <v>696.627465616338</v>
       </c>
-      <c r="O56" s="0" t="n">
+      <c r="Q56" s="0" t="n">
         <v>0.309063198928643</v>
       </c>
     </row>
@@ -10002,18 +7882,24 @@
         <v>600</v>
       </c>
       <c r="J57" s="0" t="n">
+        <v>3001</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <v>1501</v>
+      </c>
+      <c r="L57" s="0" t="n">
         <v>2067.42872491427</v>
       </c>
-      <c r="K57" s="0" t="n">
+      <c r="M57" s="0" t="n">
         <v>0.22392793139993</v>
       </c>
-      <c r="M57" s="0" t="n">
+      <c r="O57" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="N57" s="0" t="n">
+      <c r="P57" s="0" t="n">
         <v>772.806145217572</v>
       </c>
-      <c r="O57" s="0" t="n">
+      <c r="Q57" s="0" t="n">
         <v>0.28580326386727</v>
       </c>
     </row>
@@ -10040,18 +7926,24 @@
         <v>650</v>
       </c>
       <c r="J58" s="0" t="n">
+        <v>3251</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>1621</v>
+      </c>
+      <c r="L58" s="0" t="n">
         <v>2175.41215308844</v>
       </c>
-      <c r="K58" s="0" t="n">
+      <c r="M58" s="0" t="n">
         <v>0.205834779494785</v>
       </c>
-      <c r="M58" s="0" t="n">
+      <c r="O58" s="0" t="n">
         <v>650</v>
       </c>
-      <c r="N58" s="0" t="n">
+      <c r="P58" s="0" t="n">
         <v>805.845856011652</v>
       </c>
-      <c r="O58" s="0" t="n">
+      <c r="Q58" s="0" t="n">
         <v>0.267808972636776</v>
       </c>
     </row>
@@ -10078,18 +7970,24 @@
         <v>700</v>
       </c>
       <c r="J59" s="0" t="n">
+        <v>3501</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <v>1751</v>
+      </c>
+      <c r="L59" s="0" t="n">
         <v>2308.71035744086</v>
       </c>
-      <c r="K59" s="0" t="n">
+      <c r="M59" s="0" t="n">
         <v>0.215156700931377</v>
       </c>
-      <c r="M59" s="0" t="n">
+      <c r="O59" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="N59" s="0" t="n">
+      <c r="P59" s="0" t="n">
         <v>882.740871570471</v>
       </c>
-      <c r="O59" s="0" t="n">
+      <c r="Q59" s="0" t="n">
         <v>0.254642811164412</v>
       </c>
     </row>
@@ -10116,18 +8014,24 @@
         <v>750</v>
       </c>
       <c r="J60" s="0" t="n">
+        <v>3751</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <v>1871</v>
+      </c>
+      <c r="L60" s="0" t="n">
         <v>2408.50395588857</v>
       </c>
-      <c r="K60" s="0" t="n">
+      <c r="M60" s="0" t="n">
         <v>0.210131253750348</v>
       </c>
-      <c r="M60" s="0" t="n">
+      <c r="O60" s="0" t="n">
         <v>750</v>
       </c>
-      <c r="N60" s="0" t="n">
+      <c r="P60" s="0" t="n">
         <v>892.100722151325</v>
       </c>
-      <c r="O60" s="0" t="n">
+      <c r="Q60" s="0" t="n">
         <v>0.2660252427956</v>
       </c>
     </row>
@@ -10154,18 +8058,24 @@
         <v>800</v>
       </c>
       <c r="J61" s="0" t="n">
+        <v>4001</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="L61" s="0" t="n">
         <v>2591.11926901876</v>
       </c>
-      <c r="K61" s="0" t="n">
+      <c r="M61" s="0" t="n">
         <v>0.182102502906862</v>
       </c>
-      <c r="M61" s="0" t="n">
+      <c r="O61" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="N61" s="0" t="n">
+      <c r="P61" s="0" t="n">
         <v>826.838214050031</v>
       </c>
-      <c r="O61" s="0" t="n">
+      <c r="Q61" s="0" t="n">
         <v>0.248852731907704</v>
       </c>
     </row>
@@ -10192,18 +8102,24 @@
         <v>850</v>
       </c>
       <c r="J62" s="0" t="n">
+        <v>4251</v>
+      </c>
+      <c r="K62" s="0" t="n">
+        <v>2121</v>
+      </c>
+      <c r="L62" s="0" t="n">
         <v>2907.32613443273</v>
       </c>
-      <c r="K62" s="0" t="n">
+      <c r="M62" s="0" t="n">
         <v>0.175067213415687</v>
       </c>
-      <c r="M62" s="0" t="n">
+      <c r="O62" s="0" t="n">
         <v>850</v>
       </c>
-      <c r="N62" s="0" t="n">
+      <c r="P62" s="0" t="n">
         <v>1044.66558142264</v>
       </c>
-      <c r="O62" s="0" t="n">
+      <c r="Q62" s="0" t="n">
         <v>0.242339574436045</v>
       </c>
     </row>
@@ -10230,18 +8146,24 @@
         <v>900</v>
       </c>
       <c r="J63" s="0" t="n">
+        <v>4501</v>
+      </c>
+      <c r="K63" s="0" t="n">
+        <v>2251</v>
+      </c>
+      <c r="L63" s="0" t="n">
         <v>3213.15662929119</v>
       </c>
-      <c r="K63" s="0" t="n">
+      <c r="M63" s="0" t="n">
         <v>0.167587704432063</v>
       </c>
-      <c r="M63" s="0" t="n">
+      <c r="O63" s="0" t="n">
         <v>900</v>
       </c>
-      <c r="N63" s="0" t="n">
+      <c r="P63" s="0" t="n">
         <v>1243.08363246114</v>
       </c>
-      <c r="O63" s="0" t="n">
+      <c r="Q63" s="0" t="n">
         <v>0.231518404378507</v>
       </c>
     </row>
@@ -10268,18 +8190,24 @@
         <v>950</v>
       </c>
       <c r="J64" s="0" t="n">
+        <v>4751</v>
+      </c>
+      <c r="K64" s="0" t="n">
+        <v>2371</v>
+      </c>
+      <c r="L64" s="0" t="n">
         <v>3226.15301186036</v>
       </c>
-      <c r="K64" s="0" t="n">
+      <c r="M64" s="0" t="n">
         <v>0.170435222217489</v>
       </c>
-      <c r="M64" s="0" t="n">
+      <c r="O64" s="0" t="n">
         <v>950</v>
       </c>
-      <c r="N64" s="0" t="n">
+      <c r="P64" s="0" t="n">
         <v>1295.51961245325</v>
       </c>
-      <c r="O64" s="0" t="n">
+      <c r="Q64" s="0" t="n">
         <v>0.223507094634429</v>
       </c>
     </row>
@@ -10306,30 +8234,36 @@
         <v>1000</v>
       </c>
       <c r="J65" s="0" t="n">
+        <v>5001</v>
+      </c>
+      <c r="K65" s="0" t="n">
+        <v>2501</v>
+      </c>
+      <c r="L65" s="0" t="n">
         <v>3248.84490838425</v>
       </c>
-      <c r="K65" s="0" t="n">
+      <c r="M65" s="0" t="n">
         <v>0.189686264518819</v>
       </c>
-      <c r="M65" s="0" t="n">
+      <c r="O65" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="N65" s="0" t="n">
+      <c r="P65" s="0" t="n">
         <v>1148.49410646982</v>
       </c>
-      <c r="O65" s="0" t="n">
+      <c r="Q65" s="0" t="n">
         <v>0.253576280676554</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E87" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="M87" s="0" t="s">
-        <v>20</v>
+      <c r="O87" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10358,15 +8292,15 @@
         <v>2</v>
       </c>
       <c r="K88" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="M88" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="O88" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="N88" s="0" t="s">
+      <c r="P88" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="O88" s="0" t="s">
+      <c r="Q88" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -10393,18 +8327,24 @@
         <v>100</v>
       </c>
       <c r="J89" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="K89" s="0" t="n">
+        <v>251</v>
+      </c>
+      <c r="L89" s="0" t="n">
         <v>305.769928971697</v>
       </c>
-      <c r="K89" s="0" t="n">
+      <c r="M89" s="0" t="n">
         <v>0.312653119877993</v>
       </c>
-      <c r="M89" s="0" t="n">
+      <c r="O89" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="N89" s="0" t="n">
+      <c r="P89" s="0" t="n">
         <v>103.494720238677</v>
       </c>
-      <c r="O89" s="0" t="n">
+      <c r="Q89" s="0" t="n">
         <v>0.398044604256309</v>
       </c>
     </row>
@@ -10431,18 +8371,24 @@
         <v>150</v>
       </c>
       <c r="J90" s="0" t="n">
+        <v>751</v>
+      </c>
+      <c r="K90" s="0" t="n">
+        <v>371</v>
+      </c>
+      <c r="L90" s="0" t="n">
         <v>466.931199458631</v>
       </c>
-      <c r="K90" s="0" t="n">
+      <c r="M90" s="0" t="n">
         <v>0.28302114215056</v>
       </c>
-      <c r="M90" s="0" t="n">
+      <c r="O90" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="N90" s="0" t="n">
+      <c r="P90" s="0" t="n">
         <v>161.990429809269</v>
       </c>
-      <c r="O90" s="0" t="n">
+      <c r="Q90" s="0" t="n">
         <v>0.348064866937491</v>
       </c>
     </row>
@@ -10469,18 +8415,24 @@
         <v>200</v>
       </c>
       <c r="J91" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="K91" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="L91" s="0" t="n">
         <v>600.581242611654</v>
       </c>
-      <c r="K91" s="0" t="n">
+      <c r="M91" s="0" t="n">
         <v>0.271871420852192</v>
       </c>
-      <c r="M91" s="0" t="n">
+      <c r="O91" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="N91" s="0" t="n">
+      <c r="P91" s="0" t="n">
         <v>192.810214544067</v>
       </c>
-      <c r="O91" s="0" t="n">
+      <c r="Q91" s="0" t="n">
         <v>0.339019225300799</v>
       </c>
     </row>
@@ -10507,18 +8459,24 @@
         <v>250</v>
       </c>
       <c r="J92" s="0" t="n">
+        <v>1251</v>
+      </c>
+      <c r="K92" s="0" t="n">
+        <v>621</v>
+      </c>
+      <c r="L92" s="0" t="n">
         <v>814.758063919752</v>
       </c>
-      <c r="K92" s="0" t="n">
+      <c r="M92" s="0" t="n">
         <v>0.245817663536841</v>
       </c>
-      <c r="M92" s="0" t="n">
+      <c r="O92" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="N92" s="0" t="n">
+      <c r="P92" s="0" t="n">
         <v>287.491706423398</v>
       </c>
-      <c r="O92" s="0" t="n">
+      <c r="Q92" s="0" t="n">
         <v>0.311283890192441</v>
       </c>
     </row>
@@ -10545,18 +8503,24 @@
         <v>300</v>
       </c>
       <c r="J93" s="0" t="n">
+        <v>1501</v>
+      </c>
+      <c r="K93" s="0" t="n">
+        <v>751</v>
+      </c>
+      <c r="L93" s="0" t="n">
         <v>1052.03854317287</v>
       </c>
-      <c r="K93" s="0" t="n">
+      <c r="M93" s="0" t="n">
         <v>0.229944683573738</v>
       </c>
-      <c r="M93" s="0" t="n">
+      <c r="O93" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="N93" s="0" t="n">
+      <c r="P93" s="0" t="n">
         <v>419.512827506846</v>
       </c>
-      <c r="O93" s="0" t="n">
+      <c r="Q93" s="0" t="n">
         <v>0.296849540946787</v>
       </c>
     </row>
@@ -10583,18 +8547,24 @@
         <v>350</v>
       </c>
       <c r="J94" s="0" t="n">
+        <v>1751</v>
+      </c>
+      <c r="K94" s="0" t="n">
+        <v>871</v>
+      </c>
+      <c r="L94" s="0" t="n">
         <v>1124.99284950306</v>
       </c>
-      <c r="K94" s="0" t="n">
+      <c r="M94" s="0" t="n">
         <v>0.236662175295081</v>
       </c>
-      <c r="M94" s="0" t="n">
+      <c r="O94" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="N94" s="0" t="n">
+      <c r="P94" s="0" t="n">
         <v>423.055158924448</v>
       </c>
-      <c r="O94" s="0" t="n">
+      <c r="Q94" s="0" t="n">
         <v>0.280897799624021</v>
       </c>
     </row>
@@ -10621,18 +8591,24 @@
         <v>400</v>
       </c>
       <c r="J95" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="K95" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="L95" s="0" t="n">
         <v>1206.63863671213</v>
       </c>
-      <c r="K95" s="0" t="n">
+      <c r="M95" s="0" t="n">
         <v>0.214425628998118</v>
       </c>
-      <c r="M95" s="0" t="n">
+      <c r="O95" s="0" t="n">
         <v>400</v>
       </c>
-      <c r="N95" s="0" t="n">
+      <c r="P95" s="0" t="n">
         <v>418.269533888814</v>
       </c>
-      <c r="O95" s="0" t="n">
+      <c r="Q95" s="0" t="n">
         <v>0.266845558909624</v>
       </c>
     </row>
@@ -10659,18 +8635,24 @@
         <v>450</v>
       </c>
       <c r="J96" s="0" t="n">
+        <v>2251</v>
+      </c>
+      <c r="K96" s="0" t="n">
+        <v>1121</v>
+      </c>
+      <c r="L96" s="0" t="n">
         <v>1557.05233674074</v>
       </c>
-      <c r="K96" s="0" t="n">
+      <c r="M96" s="0" t="n">
         <v>0.191985470815162</v>
       </c>
-      <c r="M96" s="0" t="n">
+      <c r="O96" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="N96" s="0" t="n">
+      <c r="P96" s="0" t="n">
         <v>614.088661374743</v>
       </c>
-      <c r="O96" s="0" t="n">
+      <c r="Q96" s="0" t="n">
         <v>0.232613537755233</v>
       </c>
     </row>
@@ -10697,18 +8679,24 @@
         <v>500</v>
       </c>
       <c r="J97" s="0" t="n">
+        <v>2501</v>
+      </c>
+      <c r="K97" s="0" t="n">
+        <v>1251</v>
+      </c>
+      <c r="L97" s="0" t="n">
         <v>1651.41076873964</v>
       </c>
-      <c r="K97" s="0" t="n">
+      <c r="M97" s="0" t="n">
         <v>0.205634801665679</v>
       </c>
-      <c r="M97" s="0" t="n">
+      <c r="O97" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="N97" s="0" t="n">
+      <c r="P97" s="0" t="n">
         <v>585.854118922896</v>
       </c>
-      <c r="O97" s="0" t="n">
+      <c r="Q97" s="0" t="n">
         <v>0.28364695938989</v>
       </c>
     </row>
@@ -10735,18 +8723,24 @@
         <v>550</v>
       </c>
       <c r="J98" s="0" t="n">
+        <v>2751</v>
+      </c>
+      <c r="K98" s="0" t="n">
+        <v>1371</v>
+      </c>
+      <c r="L98" s="0" t="n">
         <v>1830.78323536227</v>
       </c>
-      <c r="K98" s="0" t="n">
+      <c r="M98" s="0" t="n">
         <v>0.207651534619249</v>
       </c>
-      <c r="M98" s="0" t="n">
+      <c r="O98" s="0" t="n">
         <v>550</v>
       </c>
-      <c r="N98" s="0" t="n">
+      <c r="P98" s="0" t="n">
         <v>696.627465616338</v>
       </c>
-      <c r="O98" s="0" t="n">
+      <c r="Q98" s="0" t="n">
         <v>0.275699527761581</v>
       </c>
     </row>
@@ -10773,18 +8767,24 @@
         <v>600</v>
       </c>
       <c r="J99" s="0" t="n">
+        <v>3001</v>
+      </c>
+      <c r="K99" s="0" t="n">
+        <v>1501</v>
+      </c>
+      <c r="L99" s="0" t="n">
         <v>2067.42872491427</v>
       </c>
-      <c r="K99" s="0" t="n">
+      <c r="M99" s="0" t="n">
         <v>0.202199847903633</v>
       </c>
-      <c r="M99" s="0" t="n">
+      <c r="O99" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="N99" s="0" t="n">
+      <c r="P99" s="0" t="n">
         <v>772.806145217572</v>
       </c>
-      <c r="O99" s="0" t="n">
+      <c r="Q99" s="0" t="n">
         <v>0.256027693945715</v>
       </c>
     </row>
@@ -10811,18 +8811,24 @@
         <v>650</v>
       </c>
       <c r="J100" s="0" t="n">
+        <v>3251</v>
+      </c>
+      <c r="K100" s="0" t="n">
+        <v>1621</v>
+      </c>
+      <c r="L100" s="0" t="n">
         <v>2175.41215308844</v>
       </c>
-      <c r="K100" s="0" t="n">
+      <c r="M100" s="0" t="n">
         <v>0.186258267611667</v>
       </c>
-      <c r="M100" s="0" t="n">
+      <c r="O100" s="0" t="n">
         <v>650</v>
       </c>
-      <c r="N100" s="0" t="n">
+      <c r="P100" s="0" t="n">
         <v>805.845856011652</v>
       </c>
-      <c r="O100" s="0" t="n">
+      <c r="Q100" s="0" t="n">
         <v>0.23904525807876</v>
       </c>
     </row>
@@ -10849,18 +8855,24 @@
         <v>700</v>
       </c>
       <c r="J101" s="0" t="n">
+        <v>3501</v>
+      </c>
+      <c r="K101" s="0" t="n">
+        <v>1751</v>
+      </c>
+      <c r="L101" s="0" t="n">
         <v>2308.71035744086</v>
       </c>
-      <c r="K101" s="0" t="n">
+      <c r="M101" s="0" t="n">
         <v>0.197908173156827</v>
       </c>
-      <c r="M101" s="0" t="n">
+      <c r="O101" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="N101" s="0" t="n">
+      <c r="P101" s="0" t="n">
         <v>882.740871570471</v>
       </c>
-      <c r="O101" s="0" t="n">
+      <c r="Q101" s="0" t="n">
         <v>0.227632256971971</v>
       </c>
     </row>
@@ -10887,18 +8899,24 @@
         <v>750</v>
       </c>
       <c r="J102" s="0" t="n">
+        <v>3751</v>
+      </c>
+      <c r="K102" s="0" t="n">
+        <v>1871</v>
+      </c>
+      <c r="L102" s="0" t="n">
         <v>2408.50395588857</v>
       </c>
-      <c r="K102" s="0" t="n">
+      <c r="M102" s="0" t="n">
         <v>0.193063732242399</v>
       </c>
-      <c r="M102" s="0" t="n">
+      <c r="O102" s="0" t="n">
         <v>750</v>
       </c>
-      <c r="N102" s="0" t="n">
+      <c r="P102" s="0" t="n">
         <v>892.100722151325</v>
       </c>
-      <c r="O102" s="0" t="n">
+      <c r="Q102" s="0" t="n">
         <v>0.239293142720315</v>
       </c>
     </row>
@@ -10925,18 +8943,24 @@
         <v>800</v>
       </c>
       <c r="J103" s="0" t="n">
+        <v>4001</v>
+      </c>
+      <c r="K103" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="L103" s="0" t="n">
         <v>2591.11926901876</v>
       </c>
-      <c r="K103" s="0" t="n">
+      <c r="M103" s="0" t="n">
         <v>0.166061168812784</v>
       </c>
-      <c r="M103" s="0" t="n">
+      <c r="O103" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="N103" s="0" t="n">
+      <c r="P103" s="0" t="n">
         <v>826.838214050031</v>
       </c>
-      <c r="O103" s="0" t="n">
+      <c r="Q103" s="0" t="n">
         <v>0.223001499492725</v>
       </c>
     </row>
@@ -10963,18 +8987,24 @@
         <v>850</v>
       </c>
       <c r="J104" s="0" t="n">
+        <v>4251</v>
+      </c>
+      <c r="K104" s="0" t="n">
+        <v>2121</v>
+      </c>
+      <c r="L104" s="0" t="n">
         <v>2907.32613443273</v>
       </c>
-      <c r="K104" s="0" t="n">
+      <c r="M104" s="0" t="n">
         <v>0.159951553053873</v>
       </c>
-      <c r="M104" s="0" t="n">
+      <c r="O104" s="0" t="n">
         <v>850</v>
       </c>
-      <c r="N104" s="0" t="n">
+      <c r="P104" s="0" t="n">
         <v>1044.66558142264</v>
       </c>
-      <c r="O104" s="0" t="n">
+      <c r="Q104" s="0" t="n">
         <v>0.219049532859484</v>
       </c>
     </row>
@@ -11001,18 +9031,24 @@
         <v>900</v>
       </c>
       <c r="J105" s="0" t="n">
+        <v>4501</v>
+      </c>
+      <c r="K105" s="0" t="n">
+        <v>2251</v>
+      </c>
+      <c r="L105" s="0" t="n">
         <v>3213.15662929119</v>
       </c>
-      <c r="K105" s="0" t="n">
+      <c r="M105" s="0" t="n">
         <v>0.15309210052881</v>
       </c>
-      <c r="M105" s="0" t="n">
+      <c r="O105" s="0" t="n">
         <v>900</v>
       </c>
-      <c r="N105" s="0" t="n">
+      <c r="P105" s="0" t="n">
         <v>1243.08363246114</v>
       </c>
-      <c r="O105" s="0" t="n">
+      <c r="Q105" s="0" t="n">
         <v>0.209437268181243</v>
       </c>
     </row>
@@ -11039,18 +9075,24 @@
         <v>950</v>
       </c>
       <c r="J106" s="0" t="n">
+        <v>4751</v>
+      </c>
+      <c r="K106" s="0" t="n">
+        <v>2371</v>
+      </c>
+      <c r="L106" s="0" t="n">
         <v>3226.15301186036</v>
       </c>
-      <c r="K106" s="0" t="n">
+      <c r="M106" s="0" t="n">
         <v>0.155819528327659</v>
       </c>
-      <c r="M106" s="0" t="n">
+      <c r="O106" s="0" t="n">
         <v>950</v>
       </c>
-      <c r="N106" s="0" t="n">
+      <c r="P106" s="0" t="n">
         <v>1295.51961245325</v>
       </c>
-      <c r="O106" s="0" t="n">
+      <c r="Q106" s="0" t="n">
         <v>0.20011711079724</v>
       </c>
     </row>
@@ -11077,18 +9119,24 @@
         <v>1000</v>
       </c>
       <c r="J107" s="0" t="n">
+        <v>5001</v>
+      </c>
+      <c r="K107" s="0" t="n">
+        <v>2501</v>
+      </c>
+      <c r="L107" s="0" t="n">
         <v>3248.84490838425</v>
       </c>
-      <c r="K107" s="0" t="n">
+      <c r="M107" s="0" t="n">
         <v>0.174595246675325</v>
       </c>
-      <c r="M107" s="0" t="n">
+      <c r="O107" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="N107" s="0" t="n">
+      <c r="P107" s="0" t="n">
         <v>1148.49410646982</v>
       </c>
-      <c r="O107" s="0" t="n">
+      <c r="Q107" s="0" t="n">
         <v>0.228195896698892</v>
       </c>
     </row>

</xml_diff>